<commit_message>
Added post-peer review manuscript
</commit_message>
<xml_diff>
--- a/tables/Table_1.xlsx
+++ b/tables/Table_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Desktop\Repo\moraine-paper-2020\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Desktop\Repo\moraine-crest-or-slope\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA41EFC3-F081-4641-B52A-445AF3261364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D03D51-AAF3-4DCA-BA09-611B31BB189F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,17 +52,25 @@
   </si>
   <si>
     <r>
-      <t>SH R</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t>Outer Pleta Naua</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <t>OPN01</t>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
     </r>
     <r>
       <rPr>
@@ -71,7 +79,107 @@
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t>± SEM</t>
+      <t>Be</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>OPN02</t>
+  </si>
+  <si>
+    <t>51.68 ± 0.5</t>
+  </si>
+  <si>
+    <t>OPN03</t>
+  </si>
+  <si>
+    <t>SAL-01</t>
+  </si>
+  <si>
+    <t>47.57 ± 0.83</t>
+  </si>
+  <si>
+    <t>SAL-02</t>
+  </si>
+  <si>
+    <t>45.07 ± 0.84</t>
+  </si>
+  <si>
+    <t>SAL-03</t>
+  </si>
+  <si>
+    <t>44.07 ± 0.82</t>
+  </si>
+  <si>
+    <t>SAL-04</t>
+  </si>
+  <si>
+    <t>47.57 ± 0.84</t>
+  </si>
+  <si>
+    <t>SAL-05</t>
+  </si>
+  <si>
+    <t>48.9 ± 0.77</t>
+  </si>
+  <si>
+    <t>SAL-06</t>
+  </si>
+  <si>
+    <t>44.53 ± 0.74</t>
+  </si>
+  <si>
+    <t>SAL-07</t>
+  </si>
+  <si>
+    <t>47.43 ± 0.96</t>
+  </si>
+  <si>
+    <t>SAL-08</t>
+  </si>
+  <si>
+    <t>47.7 ± 0.9</t>
+  </si>
+  <si>
+    <t>SAL-09</t>
+  </si>
+  <si>
+    <t>44.77 ± 0.8</t>
+  </si>
+  <si>
+    <t>SAL-10</t>
+  </si>
+  <si>
+    <t>43.03 ± 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIR-11-13 </t>
+  </si>
+  <si>
+    <r>
+      <t>36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cl</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PIR-11-14 </t>
+  </si>
+  <si>
+    <t>47.6 ± 0.83</t>
+  </si>
+  <si>
+    <r>
+      <t>Soum d'Ech</t>
     </r>
     <r>
       <rPr>
@@ -81,12 +189,21 @@
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Outer Pleta Naua</t>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <t>ECH01</t>
+  </si>
+  <si>
+    <t>42.43 ± 0.98</t>
+  </si>
+  <si>
+    <t>ECH02</t>
+  </si>
+  <si>
+    <r>
+      <t>43.2</t>
     </r>
     <r>
       <rPr>
@@ -96,157 +213,6 @@
         <rFont val="Gill Sans MT"/>
         <family val="2"/>
       </rPr>
-      <t>c</t>
-    </r>
-  </si>
-  <si>
-    <t>OPN01</t>
-  </si>
-  <si>
-    <r>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Be</t>
-    </r>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>OPN02</t>
-  </si>
-  <si>
-    <t>51.68 ± 0.5</t>
-  </si>
-  <si>
-    <t>OPN03</t>
-  </si>
-  <si>
-    <t>SAL-01</t>
-  </si>
-  <si>
-    <t>47.57 ± 0.83</t>
-  </si>
-  <si>
-    <t>SAL-02</t>
-  </si>
-  <si>
-    <t>45.07 ± 0.84</t>
-  </si>
-  <si>
-    <t>SAL-03</t>
-  </si>
-  <si>
-    <t>44.07 ± 0.82</t>
-  </si>
-  <si>
-    <t>SAL-04</t>
-  </si>
-  <si>
-    <t>47.57 ± 0.84</t>
-  </si>
-  <si>
-    <t>SAL-05</t>
-  </si>
-  <si>
-    <t>48.9 ± 0.77</t>
-  </si>
-  <si>
-    <t>SAL-06</t>
-  </si>
-  <si>
-    <t>44.53 ± 0.74</t>
-  </si>
-  <si>
-    <t>SAL-07</t>
-  </si>
-  <si>
-    <t>47.43 ± 0.96</t>
-  </si>
-  <si>
-    <t>SAL-08</t>
-  </si>
-  <si>
-    <t>47.7 ± 0.9</t>
-  </si>
-  <si>
-    <t>SAL-09</t>
-  </si>
-  <si>
-    <t>44.77 ± 0.8</t>
-  </si>
-  <si>
-    <t>SAL-10</t>
-  </si>
-  <si>
-    <t>43.03 ± 0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PIR-11-13 </t>
-  </si>
-  <si>
-    <r>
-      <t>36</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>Cl</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">PIR-11-14 </t>
-  </si>
-  <si>
-    <t>47.6 ± 0.83</t>
-  </si>
-  <si>
-    <r>
-      <t>Soum d'Ech</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-  </si>
-  <si>
-    <t>ECH01</t>
-  </si>
-  <si>
-    <t>42.43 ± 0.98</t>
-  </si>
-  <si>
-    <t>ECH02</t>
-  </si>
-  <si>
-    <r>
-      <t>43.2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
       <t>f</t>
     </r>
   </si>
@@ -261,122 +227,6 @@
   </si>
   <si>
     <t>38.77 ± 1.05</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Full sample information used for exposure age calculation is provided in the Supplementary Information or is available on GitHub: https://github.com/matt-tomkins/moraine-paper-2020, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Mean of 30 SH R-values ± the Standard Error of the Mean, </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>c</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> OPN samples from Pallàs et al. (2006), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> PIR samples from Palacios et al. (2015), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ECH samples from Rodés (2008), </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Gill Sans MT"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Measurement error, see Rodés (2008).  </t>
-    </r>
   </si>
   <si>
     <r>
@@ -424,6 +274,175 @@
         <family val="2"/>
       </rPr>
       <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SH </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">R </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>± SEM</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Full sample information used for exposure age calculation is provided in the Supplementary Information or is available on GitHub: https://github.com/matt-tomkins/moraine-paper-2020, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mean of 30 SH </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-values ± the Standard Error of the Mean, </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> OPN samples from Pallàs et al. (2006), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> PIR samples from Palacios et al. (2015), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ECH samples from Rodés (2008), </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Gill Sans MT"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Measurement error, see Rodés (2008).  </t>
     </r>
   </si>
 </sst>
@@ -431,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +499,13 @@
     </font>
     <font>
       <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Gill Sans MT"/>
@@ -894,7 +920,7 @@
   <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +938,7 @@
   <sheetData>
     <row r="2" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -953,18 +979,18 @@
         <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E4" s="2">
         <v>42.636499999999998</v>
@@ -985,16 +1011,16 @@
         <v>1.6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B5" s="7"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
         <v>42.636499999999998</v>
@@ -1015,16 +1041,16 @@
         <v>2</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="1">
         <v>42.636499999999998</v>
@@ -1045,18 +1071,18 @@
         <v>1.5</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
         <v>42.4283</v>
@@ -1077,16 +1103,16 @@
         <v>1.5</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
         <v>42.427300000000002</v>
@@ -1107,16 +1133,16 @@
         <v>1.5</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2">
         <v>42.427</v>
@@ -1137,16 +1163,16 @@
         <v>1.7</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2">
         <v>42.425400000000003</v>
@@ -1167,16 +1193,16 @@
         <v>1.5</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>42.423999999999999</v>
@@ -1197,16 +1223,16 @@
         <v>1.6</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
         <v>42.423699999999997</v>
@@ -1227,16 +1253,16 @@
         <v>1.5</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2">
         <v>42.422899999999998</v>
@@ -1257,16 +1283,16 @@
         <v>1.4</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2">
         <v>42.4223</v>
@@ -1287,16 +1313,16 @@
         <v>1.4</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2">
         <v>42.421500000000002</v>
@@ -1317,16 +1343,16 @@
         <v>1.7</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2">
         <v>42.421300000000002</v>
@@ -1347,16 +1373,16 @@
         <v>1.8</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E17" s="2">
         <v>42.421300000000002</v>
@@ -1377,16 +1403,16 @@
         <v>2.1</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="1">
         <v>42.420900000000003</v>
@@ -1407,18 +1433,18 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2">
         <v>43.086300000000001</v>
@@ -1439,16 +1465,16 @@
         <v>3.6</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B20" s="7"/>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2">
         <v>43.085799999999999</v>
@@ -1463,22 +1489,22 @@
         <v>59</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J20" s="2">
         <v>43</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2">
         <v>43.086199999999998</v>
@@ -1499,16 +1525,16 @@
         <v>3.5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="19.8" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2">
         <v>43.086500000000001</v>
@@ -1529,12 +1555,12 @@
         <v>3.3</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B23" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>

</xml_diff>